<commit_message>
additional parameter chagnes to templates
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/ceao_designation/001-CEAO_Designation.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/ceao_designation/001-CEAO_Designation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\eao\beta\code\epictrack-api\src\api\templates\event_templates\ceao_designation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DCB340-421D-4E59-A9F5-2EA878901553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A14B510D-C2F4-4EB1-8069-BE0C0DBCA633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="164">
   <si>
     <t>Cell Colors</t>
   </si>
@@ -682,6 +682,30 @@
   </si>
   <si>
     <t>SetEventsStatus</t>
+  </si>
+  <si>
+    <t>{"phase_name":"CEAO's Designation Review","work_type_id": 1, "ea_act_id": 3, "event_name": "CEAO's Designation Application Received", "start_at": 1 }</t>
+  </si>
+  <si>
+    <t>{"phase_name":"CEAO's Designation Intake","work_type_id": 1, "ea_act_id": 3, "event_name": "Submission of Draft CEAO's Designation Application", "start_at": 28 }</t>
+  </si>
+  <si>
+    <t>{"phase_name":"CEAO's Designation Intake","work_type_id": 1, "ea_act_id": 3, "event_name": "Draft CEAO's Designation Application Initial Review", "start_at": 35 }</t>
+  </si>
+  <si>
+    <t>{"is_active": false}</t>
+  </si>
+  <si>
+    <t>{"work_state": "COMPLETED"}</t>
+  </si>
+  <si>
+    <t>{"work_state": "TERMINATED"}</t>
+  </si>
+  <si>
+    <t>{"work_state": "WITHDRAWN"}</t>
+  </si>
+  <si>
+    <t>{"start_date_locked": true}</t>
   </si>
 </sst>
 </file>
@@ -1553,7 +1577,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3:D4"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3019,10 +3043,10 @@
   <dimension ref="A1:G301"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3078,7 +3102,7 @@
         <v>83</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>84</v>
+        <v>156</v>
       </c>
       <c r="G2" s="3">
         <v>1</v>
@@ -3102,7 +3126,7 @@
         <v>86</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>84</v>
+        <v>157</v>
       </c>
       <c r="G3" s="3">
         <v>2</v>
@@ -3126,7 +3150,7 @@
         <v>87</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>84</v>
+        <v>158</v>
       </c>
       <c r="G4" s="3">
         <v>3</v>
@@ -3150,7 +3174,7 @@
         <v>89</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>84</v>
+        <v>159</v>
       </c>
       <c r="G5" s="3">
         <v>4</v>
@@ -3174,7 +3198,7 @@
         <v>90</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>84</v>
+        <v>159</v>
       </c>
       <c r="G6" s="3">
         <v>5</v>
@@ -3198,7 +3222,7 @@
         <v>92</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>84</v>
+        <v>162</v>
       </c>
       <c r="G7" s="3">
         <v>6</v>
@@ -3222,7 +3246,7 @@
         <v>94</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>84</v>
+        <v>159</v>
       </c>
       <c r="G8" s="3">
         <v>7</v>
@@ -3246,7 +3270,7 @@
         <v>96</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>84</v>
+        <v>163</v>
       </c>
       <c r="G9" s="3">
         <v>8</v>
@@ -3270,7 +3294,7 @@
         <v>89</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>84</v>
+        <v>159</v>
       </c>
       <c r="G10" s="3">
         <v>9</v>
@@ -3294,7 +3318,7 @@
         <v>90</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>84</v>
+        <v>159</v>
       </c>
       <c r="G11" s="3">
         <v>10</v>
@@ -3318,7 +3342,7 @@
         <v>97</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>84</v>
+        <v>161</v>
       </c>
       <c r="G12" s="3">
         <v>11</v>
@@ -3342,7 +3366,7 @@
         <v>94</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>84</v>
+        <v>159</v>
       </c>
       <c r="G13" s="3">
         <v>12</v>
@@ -3366,7 +3390,7 @@
         <v>89</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>84</v>
+        <v>159</v>
       </c>
       <c r="G14" s="3">
         <v>13</v>
@@ -3390,7 +3414,7 @@
         <v>90</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>84</v>
+        <v>159</v>
       </c>
       <c r="G15" s="3">
         <v>14</v>
@@ -3414,7 +3438,7 @@
         <v>92</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>84</v>
+        <v>162</v>
       </c>
       <c r="G16" s="3">
         <v>15</v>
@@ -3438,7 +3462,7 @@
         <v>94</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>84</v>
+        <v>159</v>
       </c>
       <c r="G17" s="3">
         <v>16</v>
@@ -3462,7 +3486,7 @@
         <v>89</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>84</v>
+        <v>159</v>
       </c>
       <c r="G18" s="3">
         <v>17</v>
@@ -3486,7 +3510,7 @@
         <v>90</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>84</v>
+        <v>159</v>
       </c>
       <c r="G19" s="3">
         <v>18</v>
@@ -3510,7 +3534,7 @@
         <v>97</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>84</v>
+        <v>161</v>
       </c>
       <c r="G20" s="3">
         <v>19</v>
@@ -3534,7 +3558,7 @@
         <v>94</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>84</v>
+        <v>159</v>
       </c>
       <c r="G21" s="3">
         <v>20</v>
@@ -3558,7 +3582,7 @@
         <v>89</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>84</v>
+        <v>159</v>
       </c>
       <c r="G22" s="3">
         <v>21</v>
@@ -3582,7 +3606,7 @@
         <v>90</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>84</v>
+        <v>159</v>
       </c>
       <c r="G23" s="3">
         <v>22</v>
@@ -3630,7 +3654,7 @@
         <v>94</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>84</v>
+        <v>159</v>
       </c>
       <c r="G25" s="3">
         <v>24</v>
@@ -3654,7 +3678,7 @@
         <v>98</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>84</v>
+        <v>160</v>
       </c>
       <c r="G26" s="3">
         <v>25</v>
@@ -3702,7 +3726,7 @@
         <v>98</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>84</v>
+        <v>160</v>
       </c>
       <c r="G28" s="3">
         <v>27</v>
@@ -3726,7 +3750,7 @@
         <v>94</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>84</v>
+        <v>159</v>
       </c>
       <c r="G29" s="3">
         <v>28</v>

</xml_diff>

<commit_message>
action configuration fix for add_event
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/ceao_designation/001-CEAO_Designation.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/ceao_designation/001-CEAO_Designation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\aot\EPIC-FLOW\epictrack-api\src\api\templates\event_templates\ceao_designation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\eao\beta\code\epictrack-api\src\api\templates\event_templates\ceao_designation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512C3EA6-1425-46EC-AEDB-A29AC63E6178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC7B9CE-765E-44D5-941D-167A6D0F4416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="2" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -679,15 +679,6 @@
     <t>SetEventsStatus</t>
   </si>
   <si>
-    <t>{"phase_name":"CEAO's Designation Review","work_type_id": 1, "ea_act_id": 3, "event_name": "CEAO's Designation Application Received", "start_at": 1 }</t>
-  </si>
-  <si>
-    <t>{"phase_name":"CEAO's Designation Intake","work_type_id": 1, "ea_act_id": 3, "event_name": "Submission of Draft CEAO's Designation Application", "start_at": 28 }</t>
-  </si>
-  <si>
-    <t>{"phase_name":"CEAO's Designation Intake","work_type_id": 1, "ea_act_id": 3, "event_name": "Draft CEAO's Designation Application Initial Review", "start_at": 35 }</t>
-  </si>
-  <si>
     <t>{"is_active": false}</t>
   </si>
   <si>
@@ -704,6 +695,15 @@
   </si>
   <si>
     <t>MultipleDays</t>
+  </si>
+  <si>
+    <t>{"phase_name":"CEAO's Designation Review","work_type_id": 3, "ea_act_id": 3, "event_name": "CEAO's Designation Application Received", "start_at": 1 }</t>
+  </si>
+  <si>
+    <t>{"phase_name":"CEAO's Designation Intake","work_type_id": 3, "ea_act_id": 3, "event_name": "Submission of Draft CEAO's Designation Application", "start_at": 28 }</t>
+  </si>
+  <si>
+    <t>{"phase_name":"CEAO's Designation Intake","work_type_id": 3, "ea_act_id": 3, "event_name": "Draft CEAO's Designation Application Initial Review", "start_at": 35 }</t>
   </si>
 </sst>
 </file>
@@ -1255,55 +1255,55 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.4">
       <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="11"/>
       <c r="C3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="12"/>
       <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" s="10"/>
       <c r="C5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:3" ht="21" x14ac:dyDescent="0.4">
       <c r="B8" s="13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:3" ht="21" x14ac:dyDescent="0.4">
       <c r="B12" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>8</v>
       </c>
@@ -1324,18 +1324,18 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" style="2" customWidth="1"/>
-    <col min="4" max="5" width="14.7109375" style="2" customWidth="1"/>
-    <col min="6" max="7" width="12.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="6.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" style="2" customWidth="1"/>
+    <col min="4" max="5" width="14.6640625" style="2" customWidth="1"/>
+    <col min="6" max="7" width="12.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1439,103 +1439,103 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B6"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B16"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B28"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B30"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B31"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38"/>
     </row>
   </sheetData>
@@ -1571,29 +1571,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E014DF34-0612-424C-AA89-DB5D1D4ABE25}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="3" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="70.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="48.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" style="2" customWidth="1"/>
-    <col min="7" max="9" width="14.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="6.6640625" style="3" customWidth="1"/>
+    <col min="2" max="3" width="10.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="70.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="48.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" style="2" customWidth="1"/>
+    <col min="7" max="9" width="14.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>29</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>30</v>
@@ -1634,7 +1634,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2384,7 +2384,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2462,7 +2462,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -2624,7 +2624,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -2813,16 +2813,16 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
-    <col min="3" max="4" width="70.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="6.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="70.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2929,7 +2929,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2965,7 +2965,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -3040,26 +3040,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A29F23-3414-4C7A-B10C-DD605B945639}">
   <dimension ref="A1:G301"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="2"/>
-    <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="70.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="70.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="12.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="70.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="70.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -3100,13 +3100,13 @@
         <v>82</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="G2" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -3124,13 +3124,13 @@
         <v>85</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="G3" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -3148,13 +3148,13 @@
         <v>86</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="G4" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -3172,13 +3172,13 @@
         <v>88</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G5" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -3196,13 +3196,13 @@
         <v>89</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G6" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -3220,13 +3220,13 @@
         <v>91</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G7" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -3244,13 +3244,13 @@
         <v>93</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G8" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -3268,13 +3268,13 @@
         <v>95</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G9" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -3292,13 +3292,13 @@
         <v>88</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G10" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -3316,13 +3316,13 @@
         <v>89</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G11" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -3340,13 +3340,13 @@
         <v>96</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G12" s="3">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -3364,13 +3364,13 @@
         <v>93</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G13" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -3388,13 +3388,13 @@
         <v>88</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G14" s="3">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -3412,13 +3412,13 @@
         <v>89</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G15" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -3436,13 +3436,13 @@
         <v>91</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G16" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -3460,13 +3460,13 @@
         <v>93</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G17" s="3">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -3484,13 +3484,13 @@
         <v>88</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G18" s="3">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -3508,13 +3508,13 @@
         <v>89</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G19" s="3">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -3532,13 +3532,13 @@
         <v>96</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G20" s="3">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -3556,13 +3556,13 @@
         <v>93</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G21" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -3580,13 +3580,13 @@
         <v>88</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G22" s="3">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -3604,13 +3604,13 @@
         <v>89</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G23" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -3634,7 +3634,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -3652,13 +3652,13 @@
         <v>93</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G25" s="3">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -3676,13 +3676,13 @@
         <v>97</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G26" s="3">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -3706,7 +3706,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -3724,13 +3724,13 @@
         <v>97</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G28" s="3">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -3748,13 +3748,13 @@
         <v>93</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G29" s="3">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -3770,7 +3770,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -3786,7 +3786,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -3802,7 +3802,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -3866,7 +3866,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -3882,7 +3882,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -3930,7 +3930,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -3946,7 +3946,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -3962,7 +3962,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -3994,7 +3994,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -4010,7 +4010,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -4026,7 +4026,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -4074,7 +4074,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -4090,7 +4090,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -4106,7 +4106,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -4122,7 +4122,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -4138,7 +4138,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -4170,7 +4170,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -4186,7 +4186,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -4202,7 +4202,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -4218,7 +4218,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -4250,7 +4250,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -4266,7 +4266,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -4282,7 +4282,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -4314,7 +4314,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -4346,7 +4346,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -4362,7 +4362,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -4378,7 +4378,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -4394,7 +4394,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -4410,7 +4410,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -4426,7 +4426,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -4442,7 +4442,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -4474,7 +4474,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -4506,7 +4506,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -4522,7 +4522,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -4554,7 +4554,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -4570,7 +4570,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -4586,7 +4586,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -4602,7 +4602,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -4618,7 +4618,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -4634,7 +4634,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -4650,7 +4650,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -4666,7 +4666,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -4698,7 +4698,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -4714,7 +4714,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -4730,7 +4730,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -4746,7 +4746,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -4762,7 +4762,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -4778,7 +4778,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -4794,7 +4794,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -4810,7 +4810,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -4826,7 +4826,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -4842,7 +4842,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -4858,7 +4858,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -4874,7 +4874,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -4890,7 +4890,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -4906,7 +4906,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -4922,7 +4922,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="3">
         <v>102</v>
       </c>
@@ -4938,7 +4938,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="3">
         <v>103</v>
       </c>
@@ -4954,7 +4954,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="3">
         <v>104</v>
       </c>
@@ -4970,7 +4970,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="3">
         <v>105</v>
       </c>
@@ -4986,7 +4986,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="3">
         <v>106</v>
       </c>
@@ -5002,7 +5002,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="3">
         <v>107</v>
       </c>
@@ -5018,7 +5018,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -5034,7 +5034,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="3">
         <v>109</v>
       </c>
@@ -5050,7 +5050,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="3">
         <v>110</v>
       </c>
@@ -5066,7 +5066,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="3">
         <v>111</v>
       </c>
@@ -5082,7 +5082,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="3">
         <v>112</v>
       </c>
@@ -5098,7 +5098,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="3">
         <v>113</v>
       </c>
@@ -5114,7 +5114,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="3">
         <v>114</v>
       </c>
@@ -5130,7 +5130,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" s="3">
         <v>115</v>
       </c>
@@ -5146,7 +5146,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" s="3">
         <v>116</v>
       </c>
@@ -5162,7 +5162,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" s="3">
         <v>117</v>
       </c>
@@ -5178,7 +5178,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" s="3">
         <v>118</v>
       </c>
@@ -5194,7 +5194,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="3">
         <v>119</v>
       </c>
@@ -5210,7 +5210,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="3">
         <v>120</v>
       </c>
@@ -5226,7 +5226,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="3">
         <v>121</v>
       </c>
@@ -5242,7 +5242,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="3">
         <v>122</v>
       </c>
@@ -5258,7 +5258,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="3">
         <v>123</v>
       </c>
@@ -5274,7 +5274,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" s="3">
         <v>124</v>
       </c>
@@ -5290,7 +5290,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" s="3">
         <v>125</v>
       </c>
@@ -5306,7 +5306,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" s="3">
         <v>126</v>
       </c>
@@ -5322,7 +5322,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" s="3">
         <v>127</v>
       </c>
@@ -5338,7 +5338,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" s="3">
         <v>128</v>
       </c>
@@ -5354,7 +5354,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="3">
         <v>129</v>
       </c>
@@ -5370,7 +5370,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" s="3">
         <v>130</v>
       </c>
@@ -5386,7 +5386,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="3">
         <v>131</v>
       </c>
@@ -5402,7 +5402,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" s="3">
         <v>132</v>
       </c>
@@ -5418,7 +5418,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" s="3">
         <v>133</v>
       </c>
@@ -5434,7 +5434,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" s="3">
         <v>134</v>
       </c>
@@ -5450,7 +5450,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" s="3">
         <v>135</v>
       </c>
@@ -5466,7 +5466,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="3">
         <v>136</v>
       </c>
@@ -5482,7 +5482,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" s="3">
         <v>137</v>
       </c>
@@ -5498,7 +5498,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="3">
         <v>138</v>
       </c>
@@ -5514,7 +5514,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="3">
         <v>139</v>
       </c>
@@ -5530,7 +5530,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" s="3">
         <v>140</v>
       </c>
@@ -5546,7 +5546,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" s="3">
         <v>141</v>
       </c>
@@ -5562,7 +5562,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="3">
         <v>142</v>
       </c>
@@ -5578,7 +5578,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" s="3">
         <v>143</v>
       </c>
@@ -5594,7 +5594,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" s="3">
         <v>144</v>
       </c>
@@ -5610,7 +5610,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" s="3">
         <v>145</v>
       </c>
@@ -5626,7 +5626,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" s="3">
         <v>146</v>
       </c>
@@ -5642,7 +5642,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" s="3">
         <v>147</v>
       </c>
@@ -5658,7 +5658,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" s="3">
         <v>148</v>
       </c>
@@ -5674,7 +5674,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" s="3">
         <v>149</v>
       </c>
@@ -5690,7 +5690,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151" s="3">
         <v>150</v>
       </c>
@@ -5706,7 +5706,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152" s="3">
         <v>151</v>
       </c>
@@ -5722,7 +5722,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" s="3">
         <v>152</v>
       </c>
@@ -5738,7 +5738,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154" s="3">
         <v>153</v>
       </c>
@@ -5754,7 +5754,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A155" s="3">
         <v>154</v>
       </c>
@@ -5770,7 +5770,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156" s="3">
         <v>155</v>
       </c>
@@ -5786,7 +5786,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157" s="3">
         <v>156</v>
       </c>
@@ -5802,7 +5802,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158" s="3">
         <v>157</v>
       </c>
@@ -5818,7 +5818,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159" s="3">
         <v>158</v>
       </c>
@@ -5834,7 +5834,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160" s="3">
         <v>159</v>
       </c>
@@ -5850,7 +5850,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A161" s="3">
         <v>160</v>
       </c>
@@ -5866,7 +5866,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A162" s="3">
         <v>161</v>
       </c>
@@ -5882,7 +5882,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A163" s="3">
         <v>162</v>
       </c>
@@ -5898,7 +5898,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A164" s="3">
         <v>163</v>
       </c>
@@ -5914,7 +5914,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A165" s="3">
         <v>164</v>
       </c>
@@ -5930,7 +5930,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A166" s="3">
         <v>165</v>
       </c>
@@ -5946,7 +5946,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A167" s="3">
         <v>166</v>
       </c>
@@ -5962,7 +5962,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A168" s="3">
         <v>167</v>
       </c>
@@ -5978,7 +5978,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A169" s="3">
         <v>168</v>
       </c>
@@ -5994,7 +5994,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A170" s="3">
         <v>169</v>
       </c>
@@ -6010,7 +6010,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A171" s="3">
         <v>170</v>
       </c>
@@ -6026,7 +6026,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A172" s="3">
         <v>171</v>
       </c>
@@ -6042,7 +6042,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A173" s="3">
         <v>172</v>
       </c>
@@ -6058,7 +6058,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A174" s="3">
         <v>173</v>
       </c>
@@ -6074,7 +6074,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A175" s="3">
         <v>174</v>
       </c>
@@ -6090,7 +6090,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A176" s="3">
         <v>175</v>
       </c>
@@ -6106,7 +6106,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A177" s="3">
         <v>176</v>
       </c>
@@ -6122,7 +6122,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A178" s="3">
         <v>177</v>
       </c>
@@ -6138,7 +6138,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A179" s="3">
         <v>178</v>
       </c>
@@ -6154,7 +6154,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A180" s="3">
         <v>179</v>
       </c>
@@ -6170,7 +6170,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A181" s="3">
         <v>180</v>
       </c>
@@ -6186,7 +6186,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A182" s="3">
         <v>181</v>
       </c>
@@ -6202,7 +6202,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A183" s="3">
         <v>182</v>
       </c>
@@ -6218,7 +6218,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A184" s="3">
         <v>183</v>
       </c>
@@ -6234,7 +6234,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A185" s="3">
         <v>184</v>
       </c>
@@ -6250,7 +6250,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A186" s="3">
         <v>185</v>
       </c>
@@ -6266,7 +6266,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A187" s="3">
         <v>186</v>
       </c>
@@ -6282,7 +6282,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A188" s="3">
         <v>187</v>
       </c>
@@ -6298,7 +6298,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A189" s="3">
         <v>188</v>
       </c>
@@ -6314,7 +6314,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A190" s="3">
         <v>189</v>
       </c>
@@ -6330,7 +6330,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A191" s="3">
         <v>190</v>
       </c>
@@ -6346,7 +6346,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A192" s="3">
         <v>191</v>
       </c>
@@ -6362,7 +6362,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A193" s="3">
         <v>192</v>
       </c>
@@ -6378,7 +6378,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A194" s="3">
         <v>193</v>
       </c>
@@ -6394,7 +6394,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A195" s="3">
         <v>194</v>
       </c>
@@ -6410,7 +6410,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A196" s="3">
         <v>195</v>
       </c>
@@ -6426,7 +6426,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A197" s="3">
         <v>196</v>
       </c>
@@ -6442,7 +6442,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A198" s="3">
         <v>197</v>
       </c>
@@ -6458,7 +6458,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A199" s="3">
         <v>198</v>
       </c>
@@ -6474,7 +6474,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A200" s="3">
         <v>199</v>
       </c>
@@ -6490,7 +6490,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A201" s="3">
         <v>200</v>
       </c>
@@ -6506,7 +6506,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A202" s="3">
         <v>201</v>
       </c>
@@ -6522,7 +6522,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A203" s="3">
         <v>202</v>
       </c>
@@ -6538,7 +6538,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A204" s="3">
         <v>203</v>
       </c>
@@ -6554,7 +6554,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A205" s="3">
         <v>204</v>
       </c>
@@ -6570,7 +6570,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A206" s="3">
         <v>205</v>
       </c>
@@ -6586,7 +6586,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A207" s="3">
         <v>206</v>
       </c>
@@ -6602,7 +6602,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A208" s="3">
         <v>207</v>
       </c>
@@ -6618,7 +6618,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A209" s="3">
         <v>208</v>
       </c>
@@ -6634,7 +6634,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A210" s="3">
         <v>209</v>
       </c>
@@ -6650,7 +6650,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A211" s="3">
         <v>210</v>
       </c>
@@ -6666,7 +6666,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A212" s="3">
         <v>211</v>
       </c>
@@ -6682,7 +6682,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A213" s="3">
         <v>212</v>
       </c>
@@ -6698,7 +6698,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A214" s="3">
         <v>213</v>
       </c>
@@ -6714,7 +6714,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A215" s="3">
         <v>214</v>
       </c>
@@ -6730,7 +6730,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A216" s="3">
         <v>215</v>
       </c>
@@ -6746,7 +6746,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A217" s="3">
         <v>216</v>
       </c>
@@ -6762,7 +6762,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A218" s="3">
         <v>217</v>
       </c>
@@ -6778,7 +6778,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A219" s="3">
         <v>218</v>
       </c>
@@ -6794,7 +6794,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A220" s="3">
         <v>219</v>
       </c>
@@ -6810,7 +6810,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A221" s="3">
         <v>220</v>
       </c>
@@ -6826,7 +6826,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A222" s="3">
         <v>221</v>
       </c>
@@ -6842,7 +6842,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A223" s="3">
         <v>222</v>
       </c>
@@ -6858,7 +6858,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A224" s="3">
         <v>223</v>
       </c>
@@ -6874,7 +6874,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A225" s="3">
         <v>224</v>
       </c>
@@ -6890,7 +6890,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A226" s="3">
         <v>225</v>
       </c>
@@ -6906,7 +6906,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A227" s="3">
         <v>226</v>
       </c>
@@ -6922,7 +6922,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A228" s="3">
         <v>227</v>
       </c>
@@ -6938,7 +6938,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A229" s="3">
         <v>228</v>
       </c>
@@ -6954,7 +6954,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A230" s="3">
         <v>229</v>
       </c>
@@ -6970,7 +6970,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A231" s="3">
         <v>230</v>
       </c>
@@ -6986,7 +6986,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A232" s="3">
         <v>231</v>
       </c>
@@ -7002,7 +7002,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A233" s="3">
         <v>232</v>
       </c>
@@ -7018,7 +7018,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A234" s="3">
         <v>233</v>
       </c>
@@ -7034,7 +7034,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A235" s="3">
         <v>234</v>
       </c>
@@ -7050,7 +7050,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A236" s="3">
         <v>235</v>
       </c>
@@ -7066,7 +7066,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A237" s="3">
         <v>236</v>
       </c>
@@ -7082,7 +7082,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A238" s="3">
         <v>237</v>
       </c>
@@ -7098,7 +7098,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A239" s="3">
         <v>238</v>
       </c>
@@ -7114,7 +7114,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A240" s="3">
         <v>239</v>
       </c>
@@ -7130,7 +7130,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A241" s="3">
         <v>240</v>
       </c>
@@ -7146,7 +7146,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A242" s="3">
         <v>241</v>
       </c>
@@ -7162,7 +7162,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A243" s="3">
         <v>242</v>
       </c>
@@ -7178,7 +7178,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A244" s="3">
         <v>243</v>
       </c>
@@ -7194,7 +7194,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A245" s="3">
         <v>244</v>
       </c>
@@ -7210,7 +7210,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A246" s="3">
         <v>245</v>
       </c>
@@ -7226,7 +7226,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A247" s="3">
         <v>246</v>
       </c>
@@ -7242,7 +7242,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A248" s="3">
         <v>247</v>
       </c>
@@ -7258,7 +7258,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A249" s="3">
         <v>248</v>
       </c>
@@ -7274,7 +7274,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A250" s="3">
         <v>249</v>
       </c>
@@ -7290,7 +7290,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A251" s="3">
         <v>250</v>
       </c>
@@ -7306,7 +7306,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A252" s="3">
         <v>251</v>
       </c>
@@ -7322,7 +7322,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A253" s="3">
         <v>252</v>
       </c>
@@ -7338,7 +7338,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A254" s="3">
         <v>253</v>
       </c>
@@ -7354,7 +7354,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A255" s="3">
         <v>254</v>
       </c>
@@ -7370,7 +7370,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A256" s="3">
         <v>255</v>
       </c>
@@ -7386,7 +7386,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A257" s="3">
         <v>256</v>
       </c>
@@ -7402,7 +7402,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A258" s="3">
         <v>257</v>
       </c>
@@ -7418,7 +7418,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A259" s="3">
         <v>258</v>
       </c>
@@ -7434,7 +7434,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A260" s="3">
         <v>259</v>
       </c>
@@ -7450,7 +7450,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A261" s="3">
         <v>260</v>
       </c>
@@ -7466,7 +7466,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A262" s="3">
         <v>261</v>
       </c>
@@ -7482,7 +7482,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A263" s="3">
         <v>262</v>
       </c>
@@ -7498,7 +7498,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A264" s="3">
         <v>263</v>
       </c>
@@ -7514,7 +7514,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A265" s="3">
         <v>264</v>
       </c>
@@ -7530,7 +7530,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A266" s="3">
         <v>265</v>
       </c>
@@ -7546,7 +7546,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A267" s="3">
         <v>266</v>
       </c>
@@ -7562,7 +7562,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A268" s="3">
         <v>267</v>
       </c>
@@ -7578,7 +7578,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A269" s="3">
         <v>268</v>
       </c>
@@ -7594,7 +7594,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A270" s="3">
         <v>269</v>
       </c>
@@ -7610,7 +7610,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A271" s="3">
         <v>270</v>
       </c>
@@ -7626,7 +7626,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A272" s="3">
         <v>271</v>
       </c>
@@ -7642,7 +7642,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A273" s="3">
         <v>272</v>
       </c>
@@ -7658,7 +7658,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A274" s="3">
         <v>273</v>
       </c>
@@ -7674,7 +7674,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A275" s="3">
         <v>274</v>
       </c>
@@ -7690,7 +7690,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A276" s="3">
         <v>275</v>
       </c>
@@ -7706,7 +7706,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A277" s="3">
         <v>276</v>
       </c>
@@ -7722,7 +7722,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A278" s="3">
         <v>277</v>
       </c>
@@ -7738,7 +7738,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A279" s="3">
         <v>278</v>
       </c>
@@ -7754,7 +7754,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A280" s="3">
         <v>279</v>
       </c>
@@ -7770,7 +7770,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A281" s="3">
         <v>280</v>
       </c>
@@ -7786,7 +7786,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A282" s="3">
         <v>281</v>
       </c>
@@ -7802,7 +7802,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A283" s="3">
         <v>282</v>
       </c>
@@ -7818,7 +7818,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A284" s="3">
         <v>283</v>
       </c>
@@ -7834,7 +7834,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A285" s="3">
         <v>284</v>
       </c>
@@ -7850,7 +7850,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A286" s="3">
         <v>285</v>
       </c>
@@ -7866,7 +7866,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A287" s="3">
         <v>286</v>
       </c>
@@ -7882,7 +7882,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A288" s="3">
         <v>287</v>
       </c>
@@ -7898,7 +7898,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A289" s="3">
         <v>288</v>
       </c>
@@ -7914,7 +7914,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A290" s="3">
         <v>289</v>
       </c>
@@ -7930,7 +7930,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A291" s="3">
         <v>290</v>
       </c>
@@ -7946,7 +7946,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A292" s="3">
         <v>291</v>
       </c>
@@ -7962,7 +7962,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A293" s="3">
         <v>292</v>
       </c>
@@ -7978,7 +7978,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A294" s="3">
         <v>293</v>
       </c>
@@ -7994,7 +7994,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A295" s="3">
         <v>294</v>
       </c>
@@ -8010,7 +8010,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A296" s="3">
         <v>295</v>
       </c>
@@ -8026,7 +8026,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A297" s="3">
         <v>296</v>
       </c>
@@ -8042,7 +8042,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A298" s="3">
         <v>297</v>
       </c>
@@ -8058,7 +8058,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A299" s="3">
         <v>298</v>
       </c>
@@ -8074,7 +8074,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A300" s="3">
         <v>299</v>
       </c>
@@ -8090,7 +8090,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A301" s="3">
         <v>300</v>
       </c>
@@ -8132,34 +8132,34 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="3.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="3.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="3.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="24.7109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="3.7109375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" style="4" customWidth="1"/>
-    <col min="12" max="12" width="3.7109375" style="4" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="4" customWidth="1"/>
-    <col min="14" max="14" width="3.7109375" style="4" customWidth="1"/>
-    <col min="15" max="15" width="30.7109375" style="4" customWidth="1"/>
-    <col min="16" max="16" width="3.7109375" style="4" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" style="4" customWidth="1"/>
-    <col min="18" max="18" width="3.7109375" style="4" customWidth="1"/>
-    <col min="19" max="19" width="14.7109375" style="4" customWidth="1"/>
-    <col min="20" max="58" width="3.7109375" style="4" customWidth="1"/>
-    <col min="59" max="59" width="8.85546875" style="4"/>
-    <col min="60" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="3.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="3.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="3.6640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="3.6640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="3.6640625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="3.6640625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="3.6640625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="30.6640625" style="4" customWidth="1"/>
+    <col min="16" max="16" width="3.6640625" style="4" customWidth="1"/>
+    <col min="17" max="17" width="14.6640625" style="4" customWidth="1"/>
+    <col min="18" max="18" width="3.6640625" style="4" customWidth="1"/>
+    <col min="19" max="19" width="14.6640625" style="4" customWidth="1"/>
+    <col min="20" max="58" width="3.6640625" style="4" customWidth="1"/>
+    <col min="59" max="59" width="8.88671875" style="4"/>
+    <col min="60" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="1" t="s">
         <v>11</v>
@@ -8238,7 +8238,7 @@
       <c r="BF2" s="5"/>
       <c r="BG2" s="5"/>
     </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>105</v>
       </c>
@@ -8270,7 +8270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>108</v>
       </c>
@@ -8302,7 +8302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
@@ -8325,7 +8325,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>115</v>
       </c>
@@ -8342,7 +8342,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>119</v>
       </c>
@@ -8359,7 +8359,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>122</v>
       </c>
@@ -8376,7 +8376,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>125</v>
       </c>
@@ -8393,7 +8393,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>129</v>
       </c>
@@ -8407,7 +8407,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>131</v>
       </c>
@@ -8419,7 +8419,7 @@
       </c>
       <c r="O11" s="9"/>
     </row>
-    <row r="12" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>132</v>
       </c>
@@ -8431,7 +8431,7 @@
       </c>
       <c r="O12" s="9"/>
     </row>
-    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>133</v>
       </c>
@@ -8443,7 +8443,7 @@
       </c>
       <c r="O13" s="9"/>
     </row>
-    <row r="14" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>135</v>
       </c>
@@ -8455,7 +8455,7 @@
       </c>
       <c r="O14" s="9"/>
     </row>
-    <row r="15" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>137</v>
       </c>
@@ -8467,7 +8467,7 @@
       </c>
       <c r="O15" s="9"/>
     </row>
-    <row r="16" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>44</v>
       </c>
@@ -8478,7 +8478,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H17" s="4" t="s">
         <v>40</v>
       </c>
@@ -8486,7 +8486,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H18" s="4" t="s">
         <v>40</v>
       </c>
@@ -8494,7 +8494,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H19" s="4" t="s">
         <v>40</v>
       </c>
@@ -8502,7 +8502,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H20" s="4" t="s">
         <v>40</v>
       </c>
@@ -8510,7 +8510,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="21" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H21" s="4" t="s">
         <v>40</v>
       </c>
@@ -8518,7 +8518,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H22" s="4" t="s">
         <v>40</v>
       </c>
@@ -8526,7 +8526,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H23" s="4" t="s">
         <v>40</v>
       </c>
@@ -8534,7 +8534,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="24" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H24" s="4" t="s">
         <v>40</v>
       </c>
@@ -8542,7 +8542,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="25" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H25" s="4" t="s">
         <v>40</v>
       </c>
@@ -8550,7 +8550,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H26" s="4" t="s">
         <v>120</v>
       </c>
@@ -8558,7 +8558,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="27" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H27" s="4" t="s">
         <v>120</v>
       </c>
@@ -8566,7 +8566,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H28" s="4" t="s">
         <v>120</v>
       </c>
@@ -8574,7 +8574,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="29" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H29" s="4" t="s">
         <v>120</v>
       </c>
@@ -8582,7 +8582,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H30" s="4" t="s">
         <v>54</v>
       </c>
@@ -8590,7 +8590,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H31" s="4" t="s">
         <v>54</v>
       </c>
@@ -8598,7 +8598,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H32" s="4" t="s">
         <v>54</v>
       </c>
@@ -8606,7 +8606,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H33" s="4" t="s">
         <v>54</v>
       </c>
@@ -8614,7 +8614,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H34" s="4" t="s">
         <v>54</v>
       </c>
@@ -8622,7 +8622,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H35" s="4" t="s">
         <v>117</v>
       </c>
@@ -8630,7 +8630,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H36" s="4" t="s">
         <v>117</v>
       </c>
@@ -8638,7 +8638,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H37" s="4" t="s">
         <v>117</v>
       </c>
@@ -8646,7 +8646,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H38" s="4" t="s">
         <v>117</v>
       </c>
@@ -8654,7 +8654,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H39" s="4" t="s">
         <v>117</v>
       </c>

</xml_diff>

<commit_message>
Configuration fixes for the action add_event in the template files (#1199)
* project notification template updated + master templates added

* action configuration fix for add_event
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/ceao_designation/001-CEAO_Designation.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/ceao_designation/001-CEAO_Designation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\aot\EPIC-FLOW\epictrack-api\src\api\templates\event_templates\ceao_designation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\eao\beta\code\epictrack-api\src\api\templates\event_templates\ceao_designation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512C3EA6-1425-46EC-AEDB-A29AC63E6178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC7B9CE-765E-44D5-941D-167A6D0F4416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="2" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -679,15 +679,6 @@
     <t>SetEventsStatus</t>
   </si>
   <si>
-    <t>{"phase_name":"CEAO's Designation Review","work_type_id": 1, "ea_act_id": 3, "event_name": "CEAO's Designation Application Received", "start_at": 1 }</t>
-  </si>
-  <si>
-    <t>{"phase_name":"CEAO's Designation Intake","work_type_id": 1, "ea_act_id": 3, "event_name": "Submission of Draft CEAO's Designation Application", "start_at": 28 }</t>
-  </si>
-  <si>
-    <t>{"phase_name":"CEAO's Designation Intake","work_type_id": 1, "ea_act_id": 3, "event_name": "Draft CEAO's Designation Application Initial Review", "start_at": 35 }</t>
-  </si>
-  <si>
     <t>{"is_active": false}</t>
   </si>
   <si>
@@ -704,6 +695,15 @@
   </si>
   <si>
     <t>MultipleDays</t>
+  </si>
+  <si>
+    <t>{"phase_name":"CEAO's Designation Review","work_type_id": 3, "ea_act_id": 3, "event_name": "CEAO's Designation Application Received", "start_at": 1 }</t>
+  </si>
+  <si>
+    <t>{"phase_name":"CEAO's Designation Intake","work_type_id": 3, "ea_act_id": 3, "event_name": "Submission of Draft CEAO's Designation Application", "start_at": 28 }</t>
+  </si>
+  <si>
+    <t>{"phase_name":"CEAO's Designation Intake","work_type_id": 3, "ea_act_id": 3, "event_name": "Draft CEAO's Designation Application Initial Review", "start_at": 35 }</t>
   </si>
 </sst>
 </file>
@@ -1255,55 +1255,55 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.4">
       <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="11"/>
       <c r="C3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="12"/>
       <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" s="10"/>
       <c r="C5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:3" ht="21" x14ac:dyDescent="0.4">
       <c r="B8" s="13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:3" ht="21" x14ac:dyDescent="0.4">
       <c r="B12" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>8</v>
       </c>
@@ -1324,18 +1324,18 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" style="2" customWidth="1"/>
-    <col min="4" max="5" width="14.7109375" style="2" customWidth="1"/>
-    <col min="6" max="7" width="12.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="6.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" style="2" customWidth="1"/>
+    <col min="4" max="5" width="14.6640625" style="2" customWidth="1"/>
+    <col min="6" max="7" width="12.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1439,103 +1439,103 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B6"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B16"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B28"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B30"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B31"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38"/>
     </row>
   </sheetData>
@@ -1571,29 +1571,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E014DF34-0612-424C-AA89-DB5D1D4ABE25}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="3" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="70.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="48.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" style="2" customWidth="1"/>
-    <col min="7" max="9" width="14.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="6.6640625" style="3" customWidth="1"/>
+    <col min="2" max="3" width="10.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="70.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="48.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" style="2" customWidth="1"/>
+    <col min="7" max="9" width="14.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>29</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>30</v>
@@ -1634,7 +1634,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2384,7 +2384,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2462,7 +2462,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -2624,7 +2624,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -2813,16 +2813,16 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
-    <col min="3" max="4" width="70.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="6.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="70.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2929,7 +2929,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2965,7 +2965,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -3040,26 +3040,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A29F23-3414-4C7A-B10C-DD605B945639}">
   <dimension ref="A1:G301"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="2"/>
-    <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="70.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="70.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="12.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="70.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="70.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -3100,13 +3100,13 @@
         <v>82</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="G2" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -3124,13 +3124,13 @@
         <v>85</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="G3" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -3148,13 +3148,13 @@
         <v>86</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="G4" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -3172,13 +3172,13 @@
         <v>88</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G5" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -3196,13 +3196,13 @@
         <v>89</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G6" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -3220,13 +3220,13 @@
         <v>91</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G7" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -3244,13 +3244,13 @@
         <v>93</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G8" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -3268,13 +3268,13 @@
         <v>95</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G9" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -3292,13 +3292,13 @@
         <v>88</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G10" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -3316,13 +3316,13 @@
         <v>89</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G11" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -3340,13 +3340,13 @@
         <v>96</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G12" s="3">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -3364,13 +3364,13 @@
         <v>93</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G13" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -3388,13 +3388,13 @@
         <v>88</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G14" s="3">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -3412,13 +3412,13 @@
         <v>89</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G15" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -3436,13 +3436,13 @@
         <v>91</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G16" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -3460,13 +3460,13 @@
         <v>93</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G17" s="3">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -3484,13 +3484,13 @@
         <v>88</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G18" s="3">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -3508,13 +3508,13 @@
         <v>89</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G19" s="3">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -3532,13 +3532,13 @@
         <v>96</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G20" s="3">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -3556,13 +3556,13 @@
         <v>93</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G21" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -3580,13 +3580,13 @@
         <v>88</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G22" s="3">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -3604,13 +3604,13 @@
         <v>89</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G23" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -3634,7 +3634,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -3652,13 +3652,13 @@
         <v>93</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G25" s="3">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -3676,13 +3676,13 @@
         <v>97</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G26" s="3">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -3706,7 +3706,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -3724,13 +3724,13 @@
         <v>97</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G28" s="3">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -3748,13 +3748,13 @@
         <v>93</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G29" s="3">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -3770,7 +3770,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -3786,7 +3786,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -3802,7 +3802,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -3866,7 +3866,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -3882,7 +3882,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -3930,7 +3930,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -3946,7 +3946,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -3962,7 +3962,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -3994,7 +3994,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -4010,7 +4010,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -4026,7 +4026,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -4074,7 +4074,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -4090,7 +4090,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -4106,7 +4106,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -4122,7 +4122,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -4138,7 +4138,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -4170,7 +4170,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -4186,7 +4186,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -4202,7 +4202,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -4218,7 +4218,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -4250,7 +4250,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -4266,7 +4266,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -4282,7 +4282,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -4314,7 +4314,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -4346,7 +4346,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -4362,7 +4362,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -4378,7 +4378,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -4394,7 +4394,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -4410,7 +4410,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -4426,7 +4426,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -4442,7 +4442,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -4474,7 +4474,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -4506,7 +4506,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -4522,7 +4522,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -4554,7 +4554,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -4570,7 +4570,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -4586,7 +4586,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -4602,7 +4602,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -4618,7 +4618,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -4634,7 +4634,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -4650,7 +4650,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -4666,7 +4666,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -4698,7 +4698,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -4714,7 +4714,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -4730,7 +4730,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -4746,7 +4746,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -4762,7 +4762,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -4778,7 +4778,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -4794,7 +4794,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -4810,7 +4810,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -4826,7 +4826,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -4842,7 +4842,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -4858,7 +4858,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -4874,7 +4874,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -4890,7 +4890,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -4906,7 +4906,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -4922,7 +4922,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="3">
         <v>102</v>
       </c>
@@ -4938,7 +4938,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="3">
         <v>103</v>
       </c>
@@ -4954,7 +4954,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="3">
         <v>104</v>
       </c>
@@ -4970,7 +4970,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="3">
         <v>105</v>
       </c>
@@ -4986,7 +4986,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="3">
         <v>106</v>
       </c>
@@ -5002,7 +5002,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="3">
         <v>107</v>
       </c>
@@ -5018,7 +5018,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -5034,7 +5034,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="3">
         <v>109</v>
       </c>
@@ -5050,7 +5050,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="3">
         <v>110</v>
       </c>
@@ -5066,7 +5066,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="3">
         <v>111</v>
       </c>
@@ -5082,7 +5082,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="3">
         <v>112</v>
       </c>
@@ -5098,7 +5098,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="3">
         <v>113</v>
       </c>
@@ -5114,7 +5114,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="3">
         <v>114</v>
       </c>
@@ -5130,7 +5130,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" s="3">
         <v>115</v>
       </c>
@@ -5146,7 +5146,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" s="3">
         <v>116</v>
       </c>
@@ -5162,7 +5162,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" s="3">
         <v>117</v>
       </c>
@@ -5178,7 +5178,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" s="3">
         <v>118</v>
       </c>
@@ -5194,7 +5194,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="3">
         <v>119</v>
       </c>
@@ -5210,7 +5210,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="3">
         <v>120</v>
       </c>
@@ -5226,7 +5226,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="3">
         <v>121</v>
       </c>
@@ -5242,7 +5242,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="3">
         <v>122</v>
       </c>
@@ -5258,7 +5258,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="3">
         <v>123</v>
       </c>
@@ -5274,7 +5274,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" s="3">
         <v>124</v>
       </c>
@@ -5290,7 +5290,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" s="3">
         <v>125</v>
       </c>
@@ -5306,7 +5306,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" s="3">
         <v>126</v>
       </c>
@@ -5322,7 +5322,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" s="3">
         <v>127</v>
       </c>
@@ -5338,7 +5338,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" s="3">
         <v>128</v>
       </c>
@@ -5354,7 +5354,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="3">
         <v>129</v>
       </c>
@@ -5370,7 +5370,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" s="3">
         <v>130</v>
       </c>
@@ -5386,7 +5386,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="3">
         <v>131</v>
       </c>
@@ -5402,7 +5402,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" s="3">
         <v>132</v>
       </c>
@@ -5418,7 +5418,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" s="3">
         <v>133</v>
       </c>
@@ -5434,7 +5434,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" s="3">
         <v>134</v>
       </c>
@@ -5450,7 +5450,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" s="3">
         <v>135</v>
       </c>
@@ -5466,7 +5466,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="3">
         <v>136</v>
       </c>
@@ -5482,7 +5482,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" s="3">
         <v>137</v>
       </c>
@@ -5498,7 +5498,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="3">
         <v>138</v>
       </c>
@@ -5514,7 +5514,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="3">
         <v>139</v>
       </c>
@@ -5530,7 +5530,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" s="3">
         <v>140</v>
       </c>
@@ -5546,7 +5546,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" s="3">
         <v>141</v>
       </c>
@@ -5562,7 +5562,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="3">
         <v>142</v>
       </c>
@@ -5578,7 +5578,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" s="3">
         <v>143</v>
       </c>
@@ -5594,7 +5594,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" s="3">
         <v>144</v>
       </c>
@@ -5610,7 +5610,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" s="3">
         <v>145</v>
       </c>
@@ -5626,7 +5626,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" s="3">
         <v>146</v>
       </c>
@@ -5642,7 +5642,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" s="3">
         <v>147</v>
       </c>
@@ -5658,7 +5658,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" s="3">
         <v>148</v>
       </c>
@@ -5674,7 +5674,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" s="3">
         <v>149</v>
       </c>
@@ -5690,7 +5690,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151" s="3">
         <v>150</v>
       </c>
@@ -5706,7 +5706,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152" s="3">
         <v>151</v>
       </c>
@@ -5722,7 +5722,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" s="3">
         <v>152</v>
       </c>
@@ -5738,7 +5738,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154" s="3">
         <v>153</v>
       </c>
@@ -5754,7 +5754,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A155" s="3">
         <v>154</v>
       </c>
@@ -5770,7 +5770,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156" s="3">
         <v>155</v>
       </c>
@@ -5786,7 +5786,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157" s="3">
         <v>156</v>
       </c>
@@ -5802,7 +5802,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158" s="3">
         <v>157</v>
       </c>
@@ -5818,7 +5818,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159" s="3">
         <v>158</v>
       </c>
@@ -5834,7 +5834,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160" s="3">
         <v>159</v>
       </c>
@@ -5850,7 +5850,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A161" s="3">
         <v>160</v>
       </c>
@@ -5866,7 +5866,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A162" s="3">
         <v>161</v>
       </c>
@@ -5882,7 +5882,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A163" s="3">
         <v>162</v>
       </c>
@@ -5898,7 +5898,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A164" s="3">
         <v>163</v>
       </c>
@@ -5914,7 +5914,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A165" s="3">
         <v>164</v>
       </c>
@@ -5930,7 +5930,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A166" s="3">
         <v>165</v>
       </c>
@@ -5946,7 +5946,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A167" s="3">
         <v>166</v>
       </c>
@@ -5962,7 +5962,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A168" s="3">
         <v>167</v>
       </c>
@@ -5978,7 +5978,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A169" s="3">
         <v>168</v>
       </c>
@@ -5994,7 +5994,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A170" s="3">
         <v>169</v>
       </c>
@@ -6010,7 +6010,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A171" s="3">
         <v>170</v>
       </c>
@@ -6026,7 +6026,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A172" s="3">
         <v>171</v>
       </c>
@@ -6042,7 +6042,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A173" s="3">
         <v>172</v>
       </c>
@@ -6058,7 +6058,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A174" s="3">
         <v>173</v>
       </c>
@@ -6074,7 +6074,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A175" s="3">
         <v>174</v>
       </c>
@@ -6090,7 +6090,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A176" s="3">
         <v>175</v>
       </c>
@@ -6106,7 +6106,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A177" s="3">
         <v>176</v>
       </c>
@@ -6122,7 +6122,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A178" s="3">
         <v>177</v>
       </c>
@@ -6138,7 +6138,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A179" s="3">
         <v>178</v>
       </c>
@@ -6154,7 +6154,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A180" s="3">
         <v>179</v>
       </c>
@@ -6170,7 +6170,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A181" s="3">
         <v>180</v>
       </c>
@@ -6186,7 +6186,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A182" s="3">
         <v>181</v>
       </c>
@@ -6202,7 +6202,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A183" s="3">
         <v>182</v>
       </c>
@@ -6218,7 +6218,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A184" s="3">
         <v>183</v>
       </c>
@@ -6234,7 +6234,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A185" s="3">
         <v>184</v>
       </c>
@@ -6250,7 +6250,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A186" s="3">
         <v>185</v>
       </c>
@@ -6266,7 +6266,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A187" s="3">
         <v>186</v>
       </c>
@@ -6282,7 +6282,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A188" s="3">
         <v>187</v>
       </c>
@@ -6298,7 +6298,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A189" s="3">
         <v>188</v>
       </c>
@@ -6314,7 +6314,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A190" s="3">
         <v>189</v>
       </c>
@@ -6330,7 +6330,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A191" s="3">
         <v>190</v>
       </c>
@@ -6346,7 +6346,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A192" s="3">
         <v>191</v>
       </c>
@@ -6362,7 +6362,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A193" s="3">
         <v>192</v>
       </c>
@@ -6378,7 +6378,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A194" s="3">
         <v>193</v>
       </c>
@@ -6394,7 +6394,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A195" s="3">
         <v>194</v>
       </c>
@@ -6410,7 +6410,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A196" s="3">
         <v>195</v>
       </c>
@@ -6426,7 +6426,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A197" s="3">
         <v>196</v>
       </c>
@@ -6442,7 +6442,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A198" s="3">
         <v>197</v>
       </c>
@@ -6458,7 +6458,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A199" s="3">
         <v>198</v>
       </c>
@@ -6474,7 +6474,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A200" s="3">
         <v>199</v>
       </c>
@@ -6490,7 +6490,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A201" s="3">
         <v>200</v>
       </c>
@@ -6506,7 +6506,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A202" s="3">
         <v>201</v>
       </c>
@@ -6522,7 +6522,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A203" s="3">
         <v>202</v>
       </c>
@@ -6538,7 +6538,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A204" s="3">
         <v>203</v>
       </c>
@@ -6554,7 +6554,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A205" s="3">
         <v>204</v>
       </c>
@@ -6570,7 +6570,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A206" s="3">
         <v>205</v>
       </c>
@@ -6586,7 +6586,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A207" s="3">
         <v>206</v>
       </c>
@@ -6602,7 +6602,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A208" s="3">
         <v>207</v>
       </c>
@@ -6618,7 +6618,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A209" s="3">
         <v>208</v>
       </c>
@@ -6634,7 +6634,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A210" s="3">
         <v>209</v>
       </c>
@@ -6650,7 +6650,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A211" s="3">
         <v>210</v>
       </c>
@@ -6666,7 +6666,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A212" s="3">
         <v>211</v>
       </c>
@@ -6682,7 +6682,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A213" s="3">
         <v>212</v>
       </c>
@@ -6698,7 +6698,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A214" s="3">
         <v>213</v>
       </c>
@@ -6714,7 +6714,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A215" s="3">
         <v>214</v>
       </c>
@@ -6730,7 +6730,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A216" s="3">
         <v>215</v>
       </c>
@@ -6746,7 +6746,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A217" s="3">
         <v>216</v>
       </c>
@@ -6762,7 +6762,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A218" s="3">
         <v>217</v>
       </c>
@@ -6778,7 +6778,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A219" s="3">
         <v>218</v>
       </c>
@@ -6794,7 +6794,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A220" s="3">
         <v>219</v>
       </c>
@@ -6810,7 +6810,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A221" s="3">
         <v>220</v>
       </c>
@@ -6826,7 +6826,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A222" s="3">
         <v>221</v>
       </c>
@@ -6842,7 +6842,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A223" s="3">
         <v>222</v>
       </c>
@@ -6858,7 +6858,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A224" s="3">
         <v>223</v>
       </c>
@@ -6874,7 +6874,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A225" s="3">
         <v>224</v>
       </c>
@@ -6890,7 +6890,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A226" s="3">
         <v>225</v>
       </c>
@@ -6906,7 +6906,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A227" s="3">
         <v>226</v>
       </c>
@@ -6922,7 +6922,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A228" s="3">
         <v>227</v>
       </c>
@@ -6938,7 +6938,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A229" s="3">
         <v>228</v>
       </c>
@@ -6954,7 +6954,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A230" s="3">
         <v>229</v>
       </c>
@@ -6970,7 +6970,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A231" s="3">
         <v>230</v>
       </c>
@@ -6986,7 +6986,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A232" s="3">
         <v>231</v>
       </c>
@@ -7002,7 +7002,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A233" s="3">
         <v>232</v>
       </c>
@@ -7018,7 +7018,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A234" s="3">
         <v>233</v>
       </c>
@@ -7034,7 +7034,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A235" s="3">
         <v>234</v>
       </c>
@@ -7050,7 +7050,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A236" s="3">
         <v>235</v>
       </c>
@@ -7066,7 +7066,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A237" s="3">
         <v>236</v>
       </c>
@@ -7082,7 +7082,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A238" s="3">
         <v>237</v>
       </c>
@@ -7098,7 +7098,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A239" s="3">
         <v>238</v>
       </c>
@@ -7114,7 +7114,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A240" s="3">
         <v>239</v>
       </c>
@@ -7130,7 +7130,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A241" s="3">
         <v>240</v>
       </c>
@@ -7146,7 +7146,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A242" s="3">
         <v>241</v>
       </c>
@@ -7162,7 +7162,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A243" s="3">
         <v>242</v>
       </c>
@@ -7178,7 +7178,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A244" s="3">
         <v>243</v>
       </c>
@@ -7194,7 +7194,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A245" s="3">
         <v>244</v>
       </c>
@@ -7210,7 +7210,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A246" s="3">
         <v>245</v>
       </c>
@@ -7226,7 +7226,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A247" s="3">
         <v>246</v>
       </c>
@@ -7242,7 +7242,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A248" s="3">
         <v>247</v>
       </c>
@@ -7258,7 +7258,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A249" s="3">
         <v>248</v>
       </c>
@@ -7274,7 +7274,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A250" s="3">
         <v>249</v>
       </c>
@@ -7290,7 +7290,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A251" s="3">
         <v>250</v>
       </c>
@@ -7306,7 +7306,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A252" s="3">
         <v>251</v>
       </c>
@@ -7322,7 +7322,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A253" s="3">
         <v>252</v>
       </c>
@@ -7338,7 +7338,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A254" s="3">
         <v>253</v>
       </c>
@@ -7354,7 +7354,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A255" s="3">
         <v>254</v>
       </c>
@@ -7370,7 +7370,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A256" s="3">
         <v>255</v>
       </c>
@@ -7386,7 +7386,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A257" s="3">
         <v>256</v>
       </c>
@@ -7402,7 +7402,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A258" s="3">
         <v>257</v>
       </c>
@@ -7418,7 +7418,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A259" s="3">
         <v>258</v>
       </c>
@@ -7434,7 +7434,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A260" s="3">
         <v>259</v>
       </c>
@@ -7450,7 +7450,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A261" s="3">
         <v>260</v>
       </c>
@@ -7466,7 +7466,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A262" s="3">
         <v>261</v>
       </c>
@@ -7482,7 +7482,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A263" s="3">
         <v>262</v>
       </c>
@@ -7498,7 +7498,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A264" s="3">
         <v>263</v>
       </c>
@@ -7514,7 +7514,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A265" s="3">
         <v>264</v>
       </c>
@@ -7530,7 +7530,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A266" s="3">
         <v>265</v>
       </c>
@@ -7546,7 +7546,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A267" s="3">
         <v>266</v>
       </c>
@@ -7562,7 +7562,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A268" s="3">
         <v>267</v>
       </c>
@@ -7578,7 +7578,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A269" s="3">
         <v>268</v>
       </c>
@@ -7594,7 +7594,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A270" s="3">
         <v>269</v>
       </c>
@@ -7610,7 +7610,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A271" s="3">
         <v>270</v>
       </c>
@@ -7626,7 +7626,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A272" s="3">
         <v>271</v>
       </c>
@@ -7642,7 +7642,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A273" s="3">
         <v>272</v>
       </c>
@@ -7658,7 +7658,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A274" s="3">
         <v>273</v>
       </c>
@@ -7674,7 +7674,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A275" s="3">
         <v>274</v>
       </c>
@@ -7690,7 +7690,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A276" s="3">
         <v>275</v>
       </c>
@@ -7706,7 +7706,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A277" s="3">
         <v>276</v>
       </c>
@@ -7722,7 +7722,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A278" s="3">
         <v>277</v>
       </c>
@@ -7738,7 +7738,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A279" s="3">
         <v>278</v>
       </c>
@@ -7754,7 +7754,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A280" s="3">
         <v>279</v>
       </c>
@@ -7770,7 +7770,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A281" s="3">
         <v>280</v>
       </c>
@@ -7786,7 +7786,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A282" s="3">
         <v>281</v>
       </c>
@@ -7802,7 +7802,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A283" s="3">
         <v>282</v>
       </c>
@@ -7818,7 +7818,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A284" s="3">
         <v>283</v>
       </c>
@@ -7834,7 +7834,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A285" s="3">
         <v>284</v>
       </c>
@@ -7850,7 +7850,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A286" s="3">
         <v>285</v>
       </c>
@@ -7866,7 +7866,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A287" s="3">
         <v>286</v>
       </c>
@@ -7882,7 +7882,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A288" s="3">
         <v>287</v>
       </c>
@@ -7898,7 +7898,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A289" s="3">
         <v>288</v>
       </c>
@@ -7914,7 +7914,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A290" s="3">
         <v>289</v>
       </c>
@@ -7930,7 +7930,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A291" s="3">
         <v>290</v>
       </c>
@@ -7946,7 +7946,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A292" s="3">
         <v>291</v>
       </c>
@@ -7962,7 +7962,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A293" s="3">
         <v>292</v>
       </c>
@@ -7978,7 +7978,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A294" s="3">
         <v>293</v>
       </c>
@@ -7994,7 +7994,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A295" s="3">
         <v>294</v>
       </c>
@@ -8010,7 +8010,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A296" s="3">
         <v>295</v>
       </c>
@@ -8026,7 +8026,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A297" s="3">
         <v>296</v>
       </c>
@@ -8042,7 +8042,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A298" s="3">
         <v>297</v>
       </c>
@@ -8058,7 +8058,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A299" s="3">
         <v>298</v>
       </c>
@@ -8074,7 +8074,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A300" s="3">
         <v>299</v>
       </c>
@@ -8090,7 +8090,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A301" s="3">
         <v>300</v>
       </c>
@@ -8132,34 +8132,34 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="3.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="3.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="3.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="24.7109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="3.7109375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" style="4" customWidth="1"/>
-    <col min="12" max="12" width="3.7109375" style="4" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="4" customWidth="1"/>
-    <col min="14" max="14" width="3.7109375" style="4" customWidth="1"/>
-    <col min="15" max="15" width="30.7109375" style="4" customWidth="1"/>
-    <col min="16" max="16" width="3.7109375" style="4" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" style="4" customWidth="1"/>
-    <col min="18" max="18" width="3.7109375" style="4" customWidth="1"/>
-    <col min="19" max="19" width="14.7109375" style="4" customWidth="1"/>
-    <col min="20" max="58" width="3.7109375" style="4" customWidth="1"/>
-    <col min="59" max="59" width="8.85546875" style="4"/>
-    <col min="60" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="3.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="3.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="3.6640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="3.6640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="3.6640625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="3.6640625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="3.6640625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="30.6640625" style="4" customWidth="1"/>
+    <col min="16" max="16" width="3.6640625" style="4" customWidth="1"/>
+    <col min="17" max="17" width="14.6640625" style="4" customWidth="1"/>
+    <col min="18" max="18" width="3.6640625" style="4" customWidth="1"/>
+    <col min="19" max="19" width="14.6640625" style="4" customWidth="1"/>
+    <col min="20" max="58" width="3.6640625" style="4" customWidth="1"/>
+    <col min="59" max="59" width="8.88671875" style="4"/>
+    <col min="60" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="1" t="s">
         <v>11</v>
@@ -8238,7 +8238,7 @@
       <c r="BF2" s="5"/>
       <c r="BG2" s="5"/>
     </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>105</v>
       </c>
@@ -8270,7 +8270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>108</v>
       </c>
@@ -8302,7 +8302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
@@ -8325,7 +8325,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>115</v>
       </c>
@@ -8342,7 +8342,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>119</v>
       </c>
@@ -8359,7 +8359,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>122</v>
       </c>
@@ -8376,7 +8376,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>125</v>
       </c>
@@ -8393,7 +8393,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>129</v>
       </c>
@@ -8407,7 +8407,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>131</v>
       </c>
@@ -8419,7 +8419,7 @@
       </c>
       <c r="O11" s="9"/>
     </row>
-    <row r="12" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>132</v>
       </c>
@@ -8431,7 +8431,7 @@
       </c>
       <c r="O12" s="9"/>
     </row>
-    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>133</v>
       </c>
@@ -8443,7 +8443,7 @@
       </c>
       <c r="O13" s="9"/>
     </row>
-    <row r="14" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>135</v>
       </c>
@@ -8455,7 +8455,7 @@
       </c>
       <c r="O14" s="9"/>
     </row>
-    <row r="15" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>137</v>
       </c>
@@ -8467,7 +8467,7 @@
       </c>
       <c r="O15" s="9"/>
     </row>
-    <row r="16" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>44</v>
       </c>
@@ -8478,7 +8478,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H17" s="4" t="s">
         <v>40</v>
       </c>
@@ -8486,7 +8486,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H18" s="4" t="s">
         <v>40</v>
       </c>
@@ -8494,7 +8494,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H19" s="4" t="s">
         <v>40</v>
       </c>
@@ -8502,7 +8502,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H20" s="4" t="s">
         <v>40</v>
       </c>
@@ -8510,7 +8510,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="21" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H21" s="4" t="s">
         <v>40</v>
       </c>
@@ -8518,7 +8518,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H22" s="4" t="s">
         <v>40</v>
       </c>
@@ -8526,7 +8526,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H23" s="4" t="s">
         <v>40</v>
       </c>
@@ -8534,7 +8534,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="24" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H24" s="4" t="s">
         <v>40</v>
       </c>
@@ -8542,7 +8542,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="25" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H25" s="4" t="s">
         <v>40</v>
       </c>
@@ -8550,7 +8550,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H26" s="4" t="s">
         <v>120</v>
       </c>
@@ -8558,7 +8558,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="27" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H27" s="4" t="s">
         <v>120</v>
       </c>
@@ -8566,7 +8566,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H28" s="4" t="s">
         <v>120</v>
       </c>
@@ -8574,7 +8574,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="29" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H29" s="4" t="s">
         <v>120</v>
       </c>
@@ -8582,7 +8582,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H30" s="4" t="s">
         <v>54</v>
       </c>
@@ -8590,7 +8590,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H31" s="4" t="s">
         <v>54</v>
       </c>
@@ -8598,7 +8598,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H32" s="4" t="s">
         <v>54</v>
       </c>
@@ -8606,7 +8606,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H33" s="4" t="s">
         <v>54</v>
       </c>
@@ -8614,7 +8614,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H34" s="4" t="s">
         <v>54</v>
       </c>
@@ -8622,7 +8622,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H35" s="4" t="s">
         <v>117</v>
       </c>
@@ -8630,7 +8630,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H36" s="4" t="s">
         <v>117</v>
       </c>
@@ -8638,7 +8638,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H37" s="4" t="s">
         <v>117</v>
       </c>
@@ -8646,7 +8646,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H38" s="4" t="s">
         <v>117</v>
       </c>
@@ -8654,7 +8654,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H39" s="4" t="s">
         <v>117</v>
       </c>

</xml_diff>

<commit_message>
ceao designation revert changes
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/ceao_designation/001-CEAO_Designation.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/ceao_designation/001-CEAO_Designation.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\ceao_designation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FA428D-0563-4AB5-9AD5-DE1D8744CC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="14400" windowHeight="12945" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -20,20 +14,7 @@
     <sheet name="Actions" sheetId="6" r:id="rId5"/>
     <sheet name="Lookups" sheetId="2" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -731,8 +712,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -779,6 +766,150 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -802,7 +933,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -811,19 +942,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="0" tint="-0.0499893185216834"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79995117038483843"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79995117038483843"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -840,7 +971,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79995117038483843"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -850,8 +981,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -874,9 +1191,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -929,7 +1488,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -937,13 +1496,73 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
         <i val="0"/>
         <color theme="0"/>
       </font>
@@ -953,31 +1572,16 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FFCCFFCC"/>
+      <color rgb="00CCFFCC"/>
     </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1235,25 +1839,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
-    <tabColor theme="9" tint="0.79995117038483843"/>
+    <tabColor theme="9" tint="0.799981688894314"/>
   </sheetPr>
   <dimension ref="B2:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="3.6328125" customWidth="1"/>
+    <col min="1" max="1" width="3.66666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="21">
+    <row r="2" ht="21" spans="2:2">
       <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
@@ -1276,59 +1881,62 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="21">
+    <row r="8" ht="21" spans="2:2">
       <c r="B8" s="19" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:2">
       <c r="B9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="21">
+    <row r="12" ht="21" spans="2:2">
       <c r="B12" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:3">
+    <row r="13" spans="2:2">
       <c r="B13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:3">
+    <row r="14" spans="2:2">
       <c r="B14" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2:G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.6328125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="50.6328125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="24.6328125" style="3" customWidth="1"/>
-    <col min="4" max="5" width="14.6328125" style="3" customWidth="1"/>
-    <col min="6" max="8" width="12.6328125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="10.6328125" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="8.90625" style="3"/>
+    <col min="1" max="1" width="6.66666666666667" style="6" customWidth="1"/>
+    <col min="2" max="2" width="50.6666666666667" style="3" customWidth="1"/>
+    <col min="3" max="3" width="24.6666666666667" style="3" customWidth="1"/>
+    <col min="4" max="5" width="14.6666666666667" style="3" customWidth="1"/>
+    <col min="6" max="8" width="12.6666666666667" style="3" customWidth="1"/>
+    <col min="9" max="9" width="10.6666666666667" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="8.88571428571429" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1">
+    <row r="1" s="2" customFormat="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -1403,7 +2011,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="18" t="s">
         <v>21</v>
@@ -1432,7 +2040,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" s="18" t="s">
         <v>21</v>
@@ -1444,37 +2052,37 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="2:2">
       <c r="B6"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="2:2">
       <c r="B7"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="2:2">
       <c r="B8"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="2:2">
       <c r="B9"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="2:2">
       <c r="B10"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="2:2">
       <c r="B11"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="2:2">
       <c r="B12"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="2:2">
       <c r="B13"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="2:2">
       <c r="B14"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="2:2">
       <c r="B15"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="2:2">
       <c r="B16"/>
     </row>
     <row r="17" spans="2:2">
@@ -1544,60 +2152,50 @@
       <c r="B38"/>
     </row>
   </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C4">
+      <formula1>Lookups!$B$3:$B$16</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4">
+      <formula1>Lookups!$D$3:$D$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F4">
+      <formula1>Lookups!$F$3:$F$4</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
-          <x14:formula1>
-            <xm:f>Lookups!$B$3:$B$16</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
-          <x14:formula1>
-            <xm:f>Lookups!$D$3:$D$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:D4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
-          <x14:formula1>
-            <xm:f>Lookups!$F$3:$F$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F4</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.6328125" style="6" customWidth="1"/>
-    <col min="2" max="3" width="10.6328125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="70.6328125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="48.6328125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="32.6328125" style="3" customWidth="1"/>
-    <col min="7" max="9" width="14.6328125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="18.6328125" style="3" customWidth="1"/>
-    <col min="11" max="12" width="14.6328125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="10.6328125" style="3" customWidth="1"/>
-    <col min="14" max="16384" width="8.90625" style="3"/>
+    <col min="1" max="1" width="6.66666666666667" style="6" customWidth="1"/>
+    <col min="2" max="3" width="10.6666666666667" style="6" customWidth="1"/>
+    <col min="4" max="4" width="70.6666666666667" style="3" customWidth="1"/>
+    <col min="5" max="5" width="48.6666666666667" style="3" customWidth="1"/>
+    <col min="6" max="6" width="32.6666666666667" style="3" customWidth="1"/>
+    <col min="7" max="9" width="14.6666666666667" style="3" customWidth="1"/>
+    <col min="10" max="10" width="18.6666666666667" style="3" customWidth="1"/>
+    <col min="11" max="12" width="14.6666666666667" style="3" customWidth="1"/>
+    <col min="13" max="13" width="10.6666666666667" style="3" customWidth="1"/>
+    <col min="14" max="16384" width="8.88571428571429" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1">
+    <row r="1" s="2" customFormat="1" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -2753,74 +3351,58 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:H29">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="END">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="between" text="END">
       <formula>NOT(ISERROR(SEARCH("END",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="START">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="between" text="START">
       <formula>NOT(ISERROR(SEARCH("START",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C29">
+      <formula1>Phases!$A$2:$A$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H29">
+      <formula1>Lookups!$Q$3:$Q$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F29">
+      <formula1>Lookups!$I$3:$I$39</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I29">
+      <formula1>Lookups!$S$3:$S$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G29">
+      <formula1>Lookups!$K$3:$K$9</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
-          <x14:formula1>
-            <xm:f>Phases!$A$2:$A$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C29</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
-          <x14:formula1>
-            <xm:f>Lookups!$Q$3:$Q$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2:H29</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000002000000}">
-          <x14:formula1>
-            <xm:f>Lookups!$I$3:$I$39</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F29</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000003000000}">
-          <x14:formula1>
-            <xm:f>Lookups!$S$3:$S$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>I2:I29</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000004000000}">
-          <x14:formula1>
-            <xm:f>Lookups!$K$3:$K$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2:G29</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="6.6328125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.6328125" style="3" customWidth="1"/>
-    <col min="3" max="4" width="70.6328125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.6328125" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="3"/>
+    <col min="1" max="1" width="6.66666666666667" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.6666666666667" style="3" customWidth="1"/>
+    <col min="3" max="4" width="70.6666666666667" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.6666666666667" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="8.88571428571429" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1">
+    <row r="1" s="2" customFormat="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -3018,46 +3600,42 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B11">
+      <formula1>Events!$A$2:$A$29</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
-          <x14:formula1>
-            <xm:f>Events!$A$2:$A$29</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B11</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:G300"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="3"/>
-    <col min="2" max="2" width="12.6328125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="70.6328125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="30.6328125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="70.6328125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.6328125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="12.6328125" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="8.90625" style="3"/>
+    <col min="1" max="1" width="8.88571428571429" style="3"/>
+    <col min="2" max="2" width="12.6666666666667" style="3" customWidth="1"/>
+    <col min="3" max="3" width="70.6666666666667" style="3" customWidth="1"/>
+    <col min="4" max="4" width="30.6666666666667" style="3" customWidth="1"/>
+    <col min="5" max="5" width="70.6666666666667" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.6666666666667" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.6666666666667" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="8.88571428571429" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1">
+    <row r="1" s="2" customFormat="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -5361,59 +5939,55 @@
       <c r="G300" s="6"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B300">
+      <formula1>Outcomes!$A$2:$A$11</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
-          <x14:formula1>
-            <xm:f>Outcomes!$A$2:$A$11</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B300</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
-    <tabColor theme="7" tint="0.79995117038483843"/>
+    <tabColor theme="7" tint="0.799981688894314"/>
   </sheetPr>
   <dimension ref="A1:BG39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.6328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="3.6328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="3.6328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="3.6328125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6328125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="24.6328125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="3.6328125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.6328125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="3.6328125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.6328125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="3.6328125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="30.6328125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="3.6328125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="14.6328125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="3.6328125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="14.6328125" style="1" customWidth="1"/>
-    <col min="20" max="58" width="3.6328125" style="1" customWidth="1"/>
-    <col min="59" max="59" width="8.90625" style="1"/>
-    <col min="60" max="16384" width="8.90625" style="3"/>
+    <col min="1" max="1" width="3.66666666666667" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6666666666667" style="1" customWidth="1"/>
+    <col min="3" max="3" width="3.66666666666667" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6666666666667" style="1" customWidth="1"/>
+    <col min="5" max="5" width="3.66666666666667" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6666666666667" style="1" customWidth="1"/>
+    <col min="7" max="7" width="3.66666666666667" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6666666666667" style="1" customWidth="1"/>
+    <col min="9" max="9" width="24.6666666666667" style="1" customWidth="1"/>
+    <col min="10" max="10" width="3.66666666666667" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.6666666666667" style="1" customWidth="1"/>
+    <col min="12" max="12" width="3.66666666666667" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6666666666667" style="1" customWidth="1"/>
+    <col min="14" max="14" width="3.66666666666667" style="1" customWidth="1"/>
+    <col min="15" max="15" width="30.6666666666667" style="1" customWidth="1"/>
+    <col min="16" max="16" width="3.66666666666667" style="1" customWidth="1"/>
+    <col min="17" max="17" width="14.6666666666667" style="1" customWidth="1"/>
+    <col min="18" max="18" width="3.66666666666667" style="1" customWidth="1"/>
+    <col min="19" max="19" width="14.6666666666667" style="1" customWidth="1"/>
+    <col min="20" max="58" width="3.66666666666667" style="1" customWidth="1"/>
+    <col min="59" max="59" width="8.88571428571429" style="1"/>
+    <col min="60" max="16384" width="8.88571428571429" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" s="1" customFormat="1"/>
-    <row r="2" spans="1:59" s="2" customFormat="1">
+    <row r="1" s="1" customFormat="1"/>
+    <row r="2" s="2" customFormat="1" spans="1:59">
       <c r="A2" s="4"/>
       <c r="B2" s="2" t="s">
         <v>11</v>
@@ -5492,7 +6066,7 @@
       <c r="BF2" s="4"/>
       <c r="BG2" s="4"/>
     </row>
-    <row r="3" spans="1:59">
+    <row r="3" spans="2:19">
       <c r="B3" s="3" t="s">
         <v>118</v>
       </c>
@@ -5524,7 +6098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:59">
+    <row r="4" spans="2:19">
       <c r="B4" s="3" t="s">
         <v>121</v>
       </c>
@@ -5556,7 +6130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:59">
+    <row r="5" spans="2:17">
       <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
@@ -5579,7 +6153,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:59">
+    <row r="6" spans="2:15">
       <c r="B6" s="3" t="s">
         <v>128</v>
       </c>
@@ -5596,7 +6170,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:59">
+    <row r="7" spans="2:15">
       <c r="B7" s="3" t="s">
         <v>132</v>
       </c>
@@ -5613,7 +6187,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:59">
+    <row r="8" spans="2:15">
       <c r="B8" s="3" t="s">
         <v>135</v>
       </c>
@@ -5630,7 +6204,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:59">
+    <row r="9" spans="2:15">
       <c r="B9" s="3" t="s">
         <v>138</v>
       </c>
@@ -5647,7 +6221,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:59">
+    <row r="10" spans="2:15">
       <c r="B10" s="3" t="s">
         <v>142</v>
       </c>
@@ -5661,7 +6235,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:59">
+    <row r="11" spans="2:15">
       <c r="B11" s="3" t="s">
         <v>144</v>
       </c>
@@ -5673,7 +6247,7 @@
       </c>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" spans="1:59">
+    <row r="12" spans="2:15">
       <c r="B12" s="3" t="s">
         <v>145</v>
       </c>
@@ -5685,7 +6259,7 @@
       </c>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" spans="1:59">
+    <row r="13" spans="2:15">
       <c r="B13" s="3" t="s">
         <v>146</v>
       </c>
@@ -5697,7 +6271,7 @@
       </c>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="1:59">
+    <row r="14" spans="2:15">
       <c r="B14" s="3" t="s">
         <v>148</v>
       </c>
@@ -5709,7 +6283,7 @@
       </c>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" spans="1:59">
+    <row r="15" spans="2:15">
       <c r="B15" s="3" t="s">
         <v>150</v>
       </c>
@@ -5721,7 +6295,7 @@
       </c>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" spans="1:59">
+    <row r="16" spans="2:9">
       <c r="B16" s="3" t="s">
         <v>48</v>
       </c>
@@ -5917,14 +6491,15 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="O3:O15">
+  <sortState ref="O3:O15">
     <sortCondition ref="O3:O15"/>
   </sortState>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H39" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H39">
       <formula1>$K$3:$K$9</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CEAO's Designation and Minister's Designation Template (#2023)
* minister's designation template

* template fixes
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/ceao_designation/001-CEAO_Designation.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/ceao_designation/001-CEAO_Designation.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\ceao_designation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BC6A26-E30E-4A72-91F9-C7D19A6DE34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="14400" windowHeight="12945" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -14,7 +20,20 @@
     <sheet name="Actions" sheetId="6" r:id="rId5"/>
     <sheet name="Lookups" sheetId="2" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -712,14 +731,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="28">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -766,150 +779,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -933,7 +802,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -942,19 +811,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.0499893185216834"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.79995117038483843"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.79995117038483843"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -971,7 +840,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.79995117038483843"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -981,194 +850,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1191,251 +874,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1488,7 +929,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1496,61 +937,25 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <color theme="0"/>
       </font>
@@ -1560,28 +965,19 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="00CCFFCC"/>
+      <color rgb="FFCCFFCC"/>
     </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1839,26 +1235,25 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
-    <tabColor theme="9" tint="0.799981688894314"/>
+    <tabColor theme="9" tint="0.79995117038483843"/>
   </sheetPr>
   <dimension ref="B2:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="3.66666666666667" customWidth="1"/>
+    <col min="1" max="1" width="3.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" ht="21" spans="2:2">
+    <row r="2" spans="2:3" ht="21">
       <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
@@ -1881,62 +1276,59 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" ht="21" spans="2:2">
+    <row r="8" spans="2:3" ht="21">
       <c r="B8" s="19" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:2">
+    <row r="9" spans="2:3">
       <c r="B9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" ht="21" spans="2:2">
+    <row r="12" spans="2:3" ht="21">
       <c r="B12" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:2">
+    <row r="13" spans="2:3">
       <c r="B13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:2">
+    <row r="14" spans="2:3">
       <c r="B14" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="G2" sqref="G2:G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="6.66666666666667" style="6" customWidth="1"/>
-    <col min="2" max="2" width="50.6666666666667" style="3" customWidth="1"/>
-    <col min="3" max="3" width="24.6666666666667" style="3" customWidth="1"/>
-    <col min="4" max="5" width="14.6666666666667" style="3" customWidth="1"/>
-    <col min="6" max="8" width="12.6666666666667" style="3" customWidth="1"/>
-    <col min="9" max="9" width="10.6666666666667" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="8.88571428571429" style="3"/>
+    <col min="1" max="1" width="6.6328125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="50.6328125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="24.6328125" style="3" customWidth="1"/>
+    <col min="4" max="5" width="14.6328125" style="3" customWidth="1"/>
+    <col min="6" max="8" width="12.6328125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="10.6328125" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="8.90625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="1" spans="1:9">
+    <row r="1" spans="1:9" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -2052,37 +1444,37 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
+    <row r="6" spans="1:9">
       <c r="B6"/>
     </row>
-    <row r="7" spans="2:2">
+    <row r="7" spans="1:9">
       <c r="B7"/>
     </row>
-    <row r="8" spans="2:2">
+    <row r="8" spans="1:9">
       <c r="B8"/>
     </row>
-    <row r="9" spans="2:2">
+    <row r="9" spans="1:9">
       <c r="B9"/>
     </row>
-    <row r="10" spans="2:2">
+    <row r="10" spans="1:9">
       <c r="B10"/>
     </row>
-    <row r="11" spans="2:2">
+    <row r="11" spans="1:9">
       <c r="B11"/>
     </row>
-    <row r="12" spans="2:2">
+    <row r="12" spans="1:9">
       <c r="B12"/>
     </row>
-    <row r="13" spans="2:2">
+    <row r="13" spans="1:9">
       <c r="B13"/>
     </row>
-    <row r="14" spans="2:2">
+    <row r="14" spans="1:9">
       <c r="B14"/>
     </row>
-    <row r="15" spans="2:2">
+    <row r="15" spans="1:9">
       <c r="B15"/>
     </row>
-    <row r="16" spans="2:2">
+    <row r="16" spans="1:9">
       <c r="B16"/>
     </row>
     <row r="17" spans="2:2">
@@ -2152,50 +1544,60 @@
       <c r="B38"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C4">
-      <formula1>Lookups!$B$3:$B$16</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4">
-      <formula1>Lookups!$D$3:$D$5</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F4">
-      <formula1>Lookups!$F$3:$F$4</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+          <x14:formula1>
+            <xm:f>Lookups!$B$3:$B$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
+          <x14:formula1>
+            <xm:f>Lookups!$D$3:$D$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
+          <x14:formula1>
+            <xm:f>Lookups!$F$3:$F$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="6.66666666666667" style="6" customWidth="1"/>
-    <col min="2" max="3" width="10.6666666666667" style="6" customWidth="1"/>
-    <col min="4" max="4" width="70.6666666666667" style="3" customWidth="1"/>
-    <col min="5" max="5" width="48.6666666666667" style="3" customWidth="1"/>
-    <col min="6" max="6" width="32.6666666666667" style="3" customWidth="1"/>
-    <col min="7" max="9" width="14.6666666666667" style="3" customWidth="1"/>
-    <col min="10" max="10" width="18.6666666666667" style="3" customWidth="1"/>
-    <col min="11" max="12" width="14.6666666666667" style="3" customWidth="1"/>
-    <col min="13" max="13" width="10.6666666666667" style="3" customWidth="1"/>
-    <col min="14" max="16384" width="8.88571428571429" style="3"/>
+    <col min="1" max="1" width="6.6328125" style="6" customWidth="1"/>
+    <col min="2" max="3" width="10.6328125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="70.6328125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="48.6328125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="32.6328125" style="3" customWidth="1"/>
+    <col min="7" max="9" width="14.6328125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="18.6328125" style="3" customWidth="1"/>
+    <col min="11" max="12" width="14.6328125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="10.6328125" style="3" customWidth="1"/>
+    <col min="14" max="16384" width="8.90625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="1" spans="1:13">
+    <row r="1" spans="1:13" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -3351,58 +2753,74 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:H29">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="between" text="END">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="END">
       <formula>NOT(ISERROR(SEARCH("END",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="between" text="START">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="START">
       <formula>NOT(ISERROR(SEARCH("START",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C29">
-      <formula1>Phases!$A$2:$A$4</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H29">
-      <formula1>Lookups!$Q$3:$Q$5</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F29">
-      <formula1>Lookups!$I$3:$I$39</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I29">
-      <formula1>Lookups!$S$3:$S$4</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G29">
-      <formula1>Lookups!$K$3:$K$9</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
+          <x14:formula1>
+            <xm:f>Phases!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C29</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
+          <x14:formula1>
+            <xm:f>Lookups!$Q$3:$Q$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H29</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000002000000}">
+          <x14:formula1>
+            <xm:f>Lookups!$I$3:$I$39</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F29</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000003000000}">
+          <x14:formula1>
+            <xm:f>Lookups!$S$3:$S$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2:I29</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000004000000}">
+          <x14:formula1>
+            <xm:f>Lookups!$K$3:$K$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G29</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="6.66666666666667" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.6666666666667" style="3" customWidth="1"/>
-    <col min="3" max="4" width="70.6666666666667" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.6666666666667" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="8.88571428571429" style="3"/>
+    <col min="1" max="1" width="6.6328125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.6328125" style="3" customWidth="1"/>
+    <col min="3" max="4" width="70.6328125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.6328125" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="8.90625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="1" spans="1:5">
+    <row r="1" spans="1:5" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -3600,42 +3018,46 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B11">
-      <formula1>Events!$A$2:$A$29</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
+          <x14:formula1>
+            <xm:f>Events!$A$2:$A$29</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B11</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G300"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
-      <selection/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.88571428571429" style="3"/>
-    <col min="2" max="2" width="12.6666666666667" style="3" customWidth="1"/>
-    <col min="3" max="3" width="70.6666666666667" style="3" customWidth="1"/>
-    <col min="4" max="4" width="30.6666666666667" style="3" customWidth="1"/>
-    <col min="5" max="5" width="70.6666666666667" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.6666666666667" style="3" customWidth="1"/>
-    <col min="7" max="7" width="12.6666666666667" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="8.88571428571429" style="3"/>
+    <col min="1" max="1" width="8.90625" style="3"/>
+    <col min="2" max="2" width="12.6328125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="70.6328125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="30.6328125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="70.6328125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.6328125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.6328125" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="8.90625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="1" spans="1:7">
+    <row r="1" spans="1:7" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -5939,55 +5361,59 @@
       <c r="G300" s="6"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B300">
-      <formula1>Outcomes!$A$2:$A$11</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
+          <x14:formula1>
+            <xm:f>Outcomes!$A$2:$A$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B300</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
-    <tabColor theme="7" tint="0.799981688894314"/>
+    <tabColor theme="7" tint="0.79995117038483843"/>
   </sheetPr>
   <dimension ref="A1:BG39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="3.66666666666667" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6666666666667" style="1" customWidth="1"/>
-    <col min="3" max="3" width="3.66666666666667" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6666666666667" style="1" customWidth="1"/>
-    <col min="5" max="5" width="3.66666666666667" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6666666666667" style="1" customWidth="1"/>
-    <col min="7" max="7" width="3.66666666666667" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6666666666667" style="1" customWidth="1"/>
-    <col min="9" max="9" width="24.6666666666667" style="1" customWidth="1"/>
-    <col min="10" max="10" width="3.66666666666667" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.6666666666667" style="1" customWidth="1"/>
-    <col min="12" max="12" width="3.66666666666667" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.6666666666667" style="1" customWidth="1"/>
-    <col min="14" max="14" width="3.66666666666667" style="1" customWidth="1"/>
-    <col min="15" max="15" width="30.6666666666667" style="1" customWidth="1"/>
-    <col min="16" max="16" width="3.66666666666667" style="1" customWidth="1"/>
-    <col min="17" max="17" width="14.6666666666667" style="1" customWidth="1"/>
-    <col min="18" max="18" width="3.66666666666667" style="1" customWidth="1"/>
-    <col min="19" max="19" width="14.6666666666667" style="1" customWidth="1"/>
-    <col min="20" max="58" width="3.66666666666667" style="1" customWidth="1"/>
-    <col min="59" max="59" width="8.88571428571429" style="1"/>
-    <col min="60" max="16384" width="8.88571428571429" style="3"/>
+    <col min="1" max="1" width="3.6328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="3.6328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="3.6328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6328125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="3.6328125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6328125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="24.6328125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="3.6328125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.6328125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="3.6328125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6328125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="3.6328125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="30.6328125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="3.6328125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="14.6328125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="3.6328125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="14.6328125" style="1" customWidth="1"/>
+    <col min="20" max="58" width="3.6328125" style="1" customWidth="1"/>
+    <col min="59" max="59" width="8.90625" style="1"/>
+    <col min="60" max="16384" width="8.90625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1"/>
-    <row r="2" s="2" customFormat="1" spans="1:59">
+    <row r="1" spans="1:59" s="1" customFormat="1"/>
+    <row r="2" spans="1:59" s="2" customFormat="1">
       <c r="A2" s="4"/>
       <c r="B2" s="2" t="s">
         <v>11</v>
@@ -6066,7 +5492,7 @@
       <c r="BF2" s="4"/>
       <c r="BG2" s="4"/>
     </row>
-    <row r="3" spans="2:19">
+    <row r="3" spans="1:59">
       <c r="B3" s="3" t="s">
         <v>118</v>
       </c>
@@ -6098,7 +5524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:19">
+    <row r="4" spans="1:59">
       <c r="B4" s="3" t="s">
         <v>121</v>
       </c>
@@ -6130,7 +5556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:17">
+    <row r="5" spans="1:59">
       <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
@@ -6153,7 +5579,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="2:15">
+    <row r="6" spans="1:59">
       <c r="B6" s="3" t="s">
         <v>128</v>
       </c>
@@ -6170,7 +5596,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="2:15">
+    <row r="7" spans="1:59">
       <c r="B7" s="3" t="s">
         <v>132</v>
       </c>
@@ -6187,7 +5613,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="2:15">
+    <row r="8" spans="1:59">
       <c r="B8" s="3" t="s">
         <v>135</v>
       </c>
@@ -6204,7 +5630,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="2:15">
+    <row r="9" spans="1:59">
       <c r="B9" s="3" t="s">
         <v>138</v>
       </c>
@@ -6221,7 +5647,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="2:15">
+    <row r="10" spans="1:59">
       <c r="B10" s="3" t="s">
         <v>142</v>
       </c>
@@ -6235,7 +5661,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="2:15">
+    <row r="11" spans="1:59">
       <c r="B11" s="3" t="s">
         <v>144</v>
       </c>
@@ -6247,7 +5673,7 @@
       </c>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" spans="2:15">
+    <row r="12" spans="1:59">
       <c r="B12" s="3" t="s">
         <v>145</v>
       </c>
@@ -6259,7 +5685,7 @@
       </c>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" spans="2:15">
+    <row r="13" spans="1:59">
       <c r="B13" s="3" t="s">
         <v>146</v>
       </c>
@@ -6271,7 +5697,7 @@
       </c>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="2:15">
+    <row r="14" spans="1:59">
       <c r="B14" s="3" t="s">
         <v>148</v>
       </c>
@@ -6283,7 +5709,7 @@
       </c>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" spans="2:15">
+    <row r="15" spans="1:59">
       <c r="B15" s="3" t="s">
         <v>150</v>
       </c>
@@ -6295,7 +5721,7 @@
       </c>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" spans="2:9">
+    <row r="16" spans="1:59">
       <c r="B16" s="3" t="s">
         <v>48</v>
       </c>
@@ -6491,15 +5917,14 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="O3:O15">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="O3:O15">
     <sortCondition ref="O3:O15"/>
   </sortState>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H39">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H39" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>$K$3:$K$9</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>